<commit_message>
add role code và sửa lại cấu trúc db
</commit_message>
<xml_diff>
--- a/RMAPI/wwwroot/templates/MauPhieuNhapKho.xlsx
+++ b/RMAPI/wwwroot/templates/MauPhieuNhapKho.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Restaurant\TL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Restaurant\restaurant-management-api\RMAPI\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3106C8EB-9B01-482F-A1EF-16A76A50E595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BA47C7-1286-4326-BEB2-4E06FAFE3A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>PHIẾU NHẬP KHO</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Số thứ tự</t>
-  </si>
-  <si>
-    <t>Kho số</t>
   </si>
   <si>
     <t>Đơn vị</t>
@@ -141,9 +138,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,6 +151,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,186 +454,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
       <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
         <v>12</v>
       </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>